<commit_message>
Update documento + programmazione attività
</commit_message>
<xml_diff>
--- a/Programmazione attività.xlsx
+++ b/Programmazione attività.xlsx
@@ -2208,10 +2208,10 @@
     </cfRule>
   </conditionalFormatting>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
-  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="3.937007874015748E-2" right="3.937007874015748E-2" top="0.15748031496062992" bottom="0.15748031496062992" header="0.31496062992125984" footer="0"/>
   <pageSetup paperSize="9" scale="86" orientation="landscape" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
   <headerFooter>
-    <oddHeader>&amp;CProgrammazione attività
+    <oddHeader>&amp;CProgrammazione attività v.2
 SDM Team</oddHeader>
   </headerFooter>
 </worksheet>

</xml_diff>

<commit_message>
Update PERT e programmazione attività
</commit_message>
<xml_diff>
--- a/Programmazione attività.xlsx
+++ b/Programmazione attività.xlsx
@@ -12,14 +12,14 @@
     <sheet name="Foglio3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Foglio1!$A$1:$I$40</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Foglio1!$A$1:$I$41</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="97">
   <si>
     <t>A</t>
   </si>
@@ -304,6 +304,12 @@
   </si>
   <si>
     <t>AH,AL,AN</t>
+  </si>
+  <si>
+    <t>J</t>
+  </si>
+  <si>
+    <t>Stesura documento finale</t>
   </si>
 </sst>
 </file>
@@ -319,7 +325,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -350,8 +356,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59996337778862885"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="16">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -566,11 +578,63 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -623,9 +687,6 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -635,7 +696,25 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -945,7 +1024,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J40"/>
+  <dimension ref="A1:J41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
@@ -993,7 +1072,7 @@
       <c r="J1" s="1"/>
     </row>
     <row r="2" spans="1:10" ht="14.25" customHeight="1" thickTop="1">
-      <c r="A2" s="19">
+      <c r="A2" s="18">
         <v>4</v>
       </c>
       <c r="B2" s="15" t="s">
@@ -1024,7 +1103,7 @@
       <c r="J2" s="1"/>
     </row>
     <row r="3" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A3" s="19">
+      <c r="A3" s="18">
         <v>6</v>
       </c>
       <c r="B3" s="15" t="s">
@@ -1055,7 +1134,7 @@
       <c r="J3" s="1"/>
     </row>
     <row r="4" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A4" s="19">
+      <c r="A4" s="18">
         <v>7</v>
       </c>
       <c r="B4" s="15" t="s">
@@ -1086,7 +1165,7 @@
       <c r="J4" s="1"/>
     </row>
     <row r="5" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A5" s="19">
+      <c r="A5" s="18">
         <v>8</v>
       </c>
       <c r="B5" s="15" t="s">
@@ -1117,7 +1196,7 @@
       <c r="J5" s="1"/>
     </row>
     <row r="6" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A6" s="19">
+      <c r="A6" s="18">
         <v>10</v>
       </c>
       <c r="B6" s="15" t="s">
@@ -1148,7 +1227,7 @@
       <c r="J6" s="1"/>
     </row>
     <row r="7" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A7" s="19">
+      <c r="A7" s="18">
         <v>11</v>
       </c>
       <c r="B7" s="15" t="s">
@@ -1179,7 +1258,7 @@
       <c r="J7" s="1"/>
     </row>
     <row r="8" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A8" s="20">
+      <c r="A8" s="19">
         <v>14</v>
       </c>
       <c r="B8" s="16" t="s">
@@ -1210,7 +1289,7 @@
       <c r="J8" s="1"/>
     </row>
     <row r="9" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A9" s="20">
+      <c r="A9" s="19">
         <v>15</v>
       </c>
       <c r="B9" s="16" t="s">
@@ -1241,7 +1320,7 @@
       <c r="J9" s="1"/>
     </row>
     <row r="10" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A10" s="20">
+      <c r="A10" s="19">
         <v>16</v>
       </c>
       <c r="B10" s="16" t="s">
@@ -1272,7 +1351,7 @@
       <c r="J10" s="1"/>
     </row>
     <row r="11" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A11" s="20">
+      <c r="A11" s="19">
         <v>17</v>
       </c>
       <c r="B11" s="16" t="s">
@@ -1303,7 +1382,7 @@
       <c r="J11" s="1"/>
     </row>
     <row r="12" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A12" s="20">
+      <c r="A12" s="19">
         <v>18</v>
       </c>
       <c r="B12" s="16" t="s">
@@ -1334,7 +1413,7 @@
       <c r="J12" s="1"/>
     </row>
     <row r="13" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A13" s="20">
+      <c r="A13" s="19">
         <v>19</v>
       </c>
       <c r="B13" s="16" t="s">
@@ -1365,7 +1444,7 @@
       <c r="J13" s="1"/>
     </row>
     <row r="14" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A14" s="20">
+      <c r="A14" s="19">
         <v>20</v>
       </c>
       <c r="B14" s="16" t="s">
@@ -1396,7 +1475,7 @@
       <c r="J14" s="1"/>
     </row>
     <row r="15" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A15" s="20">
+      <c r="A15" s="19">
         <v>21</v>
       </c>
       <c r="B15" s="16" t="s">
@@ -1427,7 +1506,7 @@
       <c r="J15" s="1"/>
     </row>
     <row r="16" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A16" s="21">
+      <c r="A16" s="20">
         <v>24</v>
       </c>
       <c r="B16" s="17" t="s">
@@ -1449,16 +1528,16 @@
         <v>35</v>
       </c>
       <c r="H16" s="12">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="I16" s="6">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="J16" s="1"/>
     </row>
     <row r="17" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A17" s="21">
+      <c r="A17" s="20">
         <v>25</v>
       </c>
       <c r="B17" s="17" t="s">
@@ -1480,16 +1559,16 @@
         <v>36</v>
       </c>
       <c r="H17" s="12">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="I17" s="6">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="J17" s="1"/>
     </row>
     <row r="18" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A18" s="21">
+      <c r="A18" s="20">
         <v>26</v>
       </c>
       <c r="B18" s="17" t="s">
@@ -1511,16 +1590,16 @@
         <v>35</v>
       </c>
       <c r="H18" s="12">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="I18" s="6">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J18" s="1"/>
     </row>
     <row r="19" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A19" s="21">
+      <c r="A19" s="20">
         <v>27</v>
       </c>
       <c r="B19" s="17" t="s">
@@ -1542,16 +1621,16 @@
         <v>36</v>
       </c>
       <c r="H19" s="12">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="I19" s="6">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J19" s="1"/>
     </row>
     <row r="20" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A20" s="21">
+      <c r="A20" s="20">
         <v>28</v>
       </c>
       <c r="B20" s="17" t="s">
@@ -1561,7 +1640,7 @@
         <v>88</v>
       </c>
       <c r="D20" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E20" s="3">
         <v>21</v>
@@ -1570,10 +1649,10 @@
         <v>92</v>
       </c>
       <c r="G20" s="12">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H20" s="12">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="I20" s="6">
         <f t="shared" si="0"/>
@@ -1582,7 +1661,7 @@
       <c r="J20" s="1"/>
     </row>
     <row r="21" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A21" s="21">
+      <c r="A21" s="20">
         <v>29</v>
       </c>
       <c r="B21" s="17" t="s">
@@ -1601,10 +1680,10 @@
         <v>5</v>
       </c>
       <c r="G21" s="12">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="H21" s="12">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="I21" s="6">
         <f t="shared" si="0"/>
@@ -1613,7 +1692,7 @@
       <c r="J21" s="1"/>
     </row>
     <row r="22" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A22" s="21">
+      <c r="A22" s="20">
         <v>30</v>
       </c>
       <c r="B22" s="17" t="s">
@@ -1632,10 +1711,10 @@
         <v>44</v>
       </c>
       <c r="G22" s="12">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H22" s="12">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I22" s="6">
         <f t="shared" si="0"/>
@@ -1644,7 +1723,7 @@
       <c r="J22" s="1"/>
     </row>
     <row r="23" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A23" s="21">
+      <c r="A23" s="20">
         <v>31</v>
       </c>
       <c r="B23" s="17" t="s">
@@ -1654,7 +1733,7 @@
         <v>42</v>
       </c>
       <c r="D23" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E23" s="3" t="s">
         <v>93</v>
@@ -1663,10 +1742,10 @@
         <v>40</v>
       </c>
       <c r="G23" s="12">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H23" s="12">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I23" s="6">
         <f t="shared" si="0"/>
@@ -1675,7 +1754,7 @@
       <c r="J23" s="1"/>
     </row>
     <row r="24" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A24" s="21">
+      <c r="A24" s="20">
         <v>32</v>
       </c>
       <c r="B24" s="17" t="s">
@@ -1685,7 +1764,7 @@
         <v>9</v>
       </c>
       <c r="D24" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E24" s="3">
         <v>25</v>
@@ -1694,19 +1773,19 @@
         <v>2</v>
       </c>
       <c r="G24" s="12">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H24" s="12">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="I24" s="6">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="J24" s="1"/>
     </row>
     <row r="25" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A25" s="21">
+      <c r="A25" s="20">
         <v>33</v>
       </c>
       <c r="B25" s="17" t="s">
@@ -1716,7 +1795,7 @@
         <v>11</v>
       </c>
       <c r="D25" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E25" s="3">
         <v>32</v>
@@ -1725,19 +1804,19 @@
         <v>8</v>
       </c>
       <c r="G25" s="12">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="H25" s="12">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I25" s="6">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="J25" s="1"/>
     </row>
     <row r="26" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A26" s="21">
+      <c r="A26" s="20">
         <v>34</v>
       </c>
       <c r="B26" s="17" t="s">
@@ -1747,7 +1826,7 @@
         <v>13</v>
       </c>
       <c r="D26" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E26" s="3">
         <v>33</v>
@@ -1756,19 +1835,19 @@
         <v>10</v>
       </c>
       <c r="G26" s="12">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="H26" s="12">
         <v>44</v>
       </c>
       <c r="I26" s="6">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="J26" s="1"/>
     </row>
     <row r="27" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A27" s="21">
+      <c r="A27" s="20">
         <v>35</v>
       </c>
       <c r="B27" s="17" t="s">
@@ -1778,7 +1857,7 @@
         <v>15</v>
       </c>
       <c r="D27" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E27" s="3">
         <v>25.27</v>
@@ -1787,19 +1866,19 @@
         <v>16</v>
       </c>
       <c r="G27" s="12">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H27" s="12">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="I27" s="6">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J27" s="1"/>
     </row>
     <row r="28" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A28" s="21">
+      <c r="A28" s="20">
         <v>36</v>
       </c>
       <c r="B28" s="17" t="s">
@@ -1809,7 +1888,7 @@
         <v>18</v>
       </c>
       <c r="D28" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E28" s="3">
         <v>35</v>
@@ -1818,19 +1897,19 @@
         <v>14</v>
       </c>
       <c r="G28" s="12">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="H28" s="12">
         <v>42</v>
       </c>
       <c r="I28" s="6">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J28" s="1"/>
     </row>
     <row r="29" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A29" s="21">
+      <c r="A29" s="20">
         <v>37</v>
       </c>
       <c r="B29" s="17" t="s">
@@ -1849,19 +1928,19 @@
         <v>17</v>
       </c>
       <c r="G29" s="12">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H29" s="12">
         <v>44</v>
       </c>
       <c r="I29" s="6">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J29" s="1"/>
     </row>
     <row r="30" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A30" s="21">
+      <c r="A30" s="20">
         <v>38</v>
       </c>
       <c r="B30" s="17" t="s">
@@ -1871,7 +1950,7 @@
         <v>22</v>
       </c>
       <c r="D30" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E30" s="3">
         <v>29</v>
@@ -1892,7 +1971,7 @@
       <c r="J30" s="1"/>
     </row>
     <row r="31" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A31" s="21">
+      <c r="A31" s="20">
         <v>39</v>
       </c>
       <c r="B31" s="17" t="s">
@@ -1902,7 +1981,7 @@
         <v>24</v>
       </c>
       <c r="D31" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E31" s="3">
         <v>38</v>
@@ -1911,10 +1990,10 @@
         <v>21</v>
       </c>
       <c r="G31" s="12">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H31" s="12">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I31" s="6">
         <f t="shared" si="0"/>
@@ -1923,7 +2002,7 @@
       <c r="J31" s="1"/>
     </row>
     <row r="32" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A32" s="21">
+      <c r="A32" s="20">
         <v>40</v>
       </c>
       <c r="B32" s="17" t="s">
@@ -1933,7 +2012,7 @@
         <v>26</v>
       </c>
       <c r="D32" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E32" s="3">
         <v>39</v>
@@ -1954,7 +2033,7 @@
       <c r="J32" s="1"/>
     </row>
     <row r="33" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A33" s="21">
+      <c r="A33" s="20">
         <v>41</v>
       </c>
       <c r="B33" s="17" t="s">
@@ -1964,7 +2043,7 @@
         <v>28</v>
       </c>
       <c r="D33" s="3">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E33" s="3">
         <v>30</v>
@@ -1973,10 +2052,10 @@
         <v>7</v>
       </c>
       <c r="G33" s="12">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="H33" s="12">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="I33" s="6">
         <f t="shared" si="0"/>
@@ -1985,7 +2064,7 @@
       <c r="J33" s="1"/>
     </row>
     <row r="34" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A34" s="21">
+      <c r="A34" s="20">
         <v>42</v>
       </c>
       <c r="B34" s="17" t="s">
@@ -1995,7 +2074,7 @@
         <v>30</v>
       </c>
       <c r="D34" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E34" s="3">
         <v>41</v>
@@ -2004,10 +2083,10 @@
         <v>27</v>
       </c>
       <c r="G34" s="12">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="H34" s="12">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="I34" s="6">
         <f t="shared" si="0"/>
@@ -2016,7 +2095,7 @@
       <c r="J34" s="1"/>
     </row>
     <row r="35" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A35" s="21">
+      <c r="A35" s="20">
         <v>43</v>
       </c>
       <c r="B35" s="17" t="s">
@@ -2026,7 +2105,7 @@
         <v>32</v>
       </c>
       <c r="D35" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E35" s="3">
         <v>42.45</v>
@@ -2035,10 +2114,10 @@
         <v>41</v>
       </c>
       <c r="G35" s="12">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="H35" s="12">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="I35" s="6">
         <f t="shared" si="0"/>
@@ -2047,7 +2126,7 @@
       <c r="J35" s="1"/>
     </row>
     <row r="36" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A36" s="21">
+      <c r="A36" s="20">
         <v>44</v>
       </c>
       <c r="B36" s="17" t="s">
@@ -2057,7 +2136,7 @@
         <v>34</v>
       </c>
       <c r="D36" s="3">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E36" s="3">
         <v>47</v>
@@ -2066,10 +2145,10 @@
         <v>45</v>
       </c>
       <c r="G36" s="12">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="H36" s="12">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="I36" s="6">
         <f t="shared" si="0"/>
@@ -2078,7 +2157,7 @@
       <c r="J36" s="1"/>
     </row>
     <row r="37" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A37" s="21">
+      <c r="A37" s="20">
         <v>45</v>
       </c>
       <c r="B37" s="17" t="s">
@@ -2088,7 +2167,7 @@
         <v>37</v>
       </c>
       <c r="D37" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E37" s="3">
         <v>41</v>
@@ -2097,19 +2176,19 @@
         <v>27</v>
       </c>
       <c r="G37" s="12">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="H37" s="12">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I37" s="6">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="J37" s="1"/>
     </row>
     <row r="38" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A38" s="21">
+      <c r="A38" s="20">
         <v>46</v>
       </c>
       <c r="B38" s="17" t="s">
@@ -2119,7 +2198,7 @@
         <v>39</v>
       </c>
       <c r="D38" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E38" s="3">
         <v>45</v>
@@ -2128,19 +2207,19 @@
         <v>36</v>
       </c>
       <c r="G38" s="12">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="H38" s="12">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="I38" s="6">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="J38" s="1"/>
     </row>
     <row r="39" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A39" s="21">
+      <c r="A39" s="20">
         <v>47</v>
       </c>
       <c r="B39" s="17" t="s">
@@ -2150,7 +2229,7 @@
         <v>43</v>
       </c>
       <c r="D39" s="3">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E39" s="3">
         <v>43.46</v>
@@ -2159,10 +2238,10 @@
         <v>35</v>
       </c>
       <c r="G39" s="12">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="H39" s="12">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="I39" s="6">
         <f t="shared" si="0"/>
@@ -2170,36 +2249,67 @@
       </c>
       <c r="J39" s="1"/>
     </row>
-    <row r="40" spans="1:10" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A40" s="22">
+    <row r="40" spans="1:10" ht="14.25" customHeight="1">
+      <c r="A40" s="23">
         <v>50</v>
       </c>
-      <c r="B40" s="18" t="s">
+      <c r="B40" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="C40" s="18" t="s">
+      <c r="C40" s="24" t="s">
         <v>52</v>
       </c>
-      <c r="D40" s="4">
-        <v>2</v>
-      </c>
-      <c r="E40" s="4">
+      <c r="D40" s="21">
+        <v>3</v>
+      </c>
+      <c r="E40" s="21">
         <v>47</v>
       </c>
-      <c r="F40" s="13" t="s">
+      <c r="F40" s="22" t="s">
         <v>45</v>
       </c>
-      <c r="G40" s="13">
+      <c r="G40" s="22">
+        <v>66</v>
+      </c>
+      <c r="H40" s="22">
+        <v>66</v>
+      </c>
+      <c r="I40" s="27">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J40" s="1"/>
+    </row>
+    <row r="41" spans="1:10" ht="14.25" customHeight="1" thickBot="1">
+      <c r="A41" s="25">
+        <v>52</v>
+      </c>
+      <c r="B41" s="26" t="s">
+        <v>95</v>
+      </c>
+      <c r="C41" s="26" t="s">
+        <v>96</v>
+      </c>
+      <c r="D41" s="4">
+        <v>5</v>
+      </c>
+      <c r="E41" s="4">
+        <v>50</v>
+      </c>
+      <c r="F41" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="G41" s="13">
         <v>71</v>
       </c>
-      <c r="H40" s="13">
+      <c r="H41" s="13">
         <v>71</v>
       </c>
-      <c r="I40" s="14">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J40" s="1"/>
+      <c r="I41" s="14">
+        <f>H41-G41</f>
+        <v>0</v>
+      </c>
+      <c r="J41" s="1"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="I1:I1048576">

</xml_diff>